<commit_message>
Add updated robot design
</commit_message>
<xml_diff>
--- a/CAD/BOM.xlsx
+++ b/CAD/BOM.xlsx
@@ -8,26 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satom\Desktop\Robot\CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAC38B8-65F0-41AA-8170-C1B6108CF65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBED62F-7FD2-4F8E-99FA-71FD4E595F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7530" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Purchase" sheetId="1" r:id="rId1"/>
     <sheet name="3D Print" sheetId="2" r:id="rId2"/>
     <sheet name="Laser Cut" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
@@ -50,21 +61,12 @@
     <t>Motor Shaft</t>
   </si>
   <si>
-    <t>Spider Coupler</t>
-  </si>
-  <si>
     <t>Ball Bearing</t>
   </si>
   <si>
-    <t>Wheel</t>
-  </si>
-  <si>
     <t>Ball Caster</t>
   </si>
   <si>
-    <t>Heat Set Inserts</t>
-  </si>
-  <si>
     <t>Plastic Standoffs</t>
   </si>
   <si>
@@ -80,26 +82,92 @@
     <t>Motor Mount</t>
   </si>
   <si>
-    <t>Hex Standoff __</t>
-  </si>
-  <si>
-    <t>Hex bolts???</t>
-  </si>
-  <si>
-    <t>Screws</t>
-  </si>
-  <si>
     <t>DigiKey</t>
   </si>
   <si>
     <t>1738-1328-ND</t>
+  </si>
+  <si>
+    <t>Shaft Coupling</t>
+  </si>
+  <si>
+    <t>https://www.dfrobot.com/product-1462.html</t>
+  </si>
+  <si>
+    <t>DFRobot</t>
+  </si>
+  <si>
+    <t>Room36</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Aluminum-Coupling-Flexible-Coupler-Connector/dp/B06Y6424Z5?th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/NONMON-Inline-Wheels-Skates-Replacement/dp/B088RDVCT1/ref=sr_1_9?crid=1OHCNY2EIAFPM&amp;keywords=80%2Bmm%2Bskate%2Bwheel&amp;qid=1701125356&amp;sprefix=80%2Bmm%2Bskatewheel%2Caps%2C125&amp;sr=8-9&amp;th=1&amp;psc=1</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Wheels</t>
+  </si>
+  <si>
+    <t>M3 Heat Set Inserts</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Threaded-Inserts-Printing-Embedment-Automotive/dp/B0BQJ6CRNJ/ref=sr_1_3?crid=5P7BZY47HOX3&amp;keywords=m3+heat+set+inserts&amp;qid=1701125622&amp;sprefix=m3+heat+s%2Caps%2C127&amp;sr=8-3</t>
+  </si>
+  <si>
+    <t>M3 Screws</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Metric-Assortment-Button-Socket-Threaded/dp/B0C7CZ6LJN/ref=sr_1_4?crid=2HO8N1AX3QFO7&amp;keywords=m3+bolts&amp;qid=1701125722&amp;sprefix=m3%2Caps%2C252&amp;sr=8-4</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/uxcell-500pcs-Spacers-Washers-Height/dp/B07FKJNQ2R/ref=sr_1_5?content-id=amzn1.sym.918a99dd-4826-4c0a-be33-a6705d69c4cf%3Aamzn1.sym.918a99dd-4826-4c0a-be33-a6705d69c4cf&amp;crid=10VDR2XAKEQI8&amp;keywords=Spacers&amp;pd_rd_r=ff50aa0e-bcc5-4ca2-9e34-4dafaf53d1b7&amp;pd_rd_w=jv4pl&amp;pd_rd_wg=xqcOH&amp;pf_rd_p=918a99dd-4826-4c0a-be33-a6705d69c4cf&amp;pf_rd_r=FYYYZSEK9MT5WGV9X1CK&amp;pid=bpmk5Iy&amp;qid=1701126121&amp;refinements=p_n_feature_twenty-three_browse-bin%3A19047481011%2Cp_n_material_browse%3A17548927011%7C17548928011%2Cp_n_feature_twenty_browse-bin%3A17420943011&amp;s=industrial&amp;sprefix=pcb%2Bstandoff%2Caps%2C124&amp;sr=1-5</t>
+  </si>
+  <si>
+    <t>Hex Standoff 3 Inches</t>
+  </si>
+  <si>
+    <t>Hex Standoff Bolts</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Standoff-Brass-Female-Plated-Length/dp/B00PKGCQZG/ref=sr_1_3?content-id=amzn1.sym.918a99dd-4826-4c0a-be33-a6705d69c4cf%3Aamzn1.sym.918a99dd-4826-4c0a-be33-a6705d69c4cf&amp;crid=10VDR2XAKEQI8&amp;keywords=Spacers&amp;pd_rd_r=9490d230-b7c2-4164-b95d-593ae935ff5c&amp;pd_rd_w=RvT9c&amp;pd_rd_wg=tnYmu&amp;pf_rd_p=918a99dd-4826-4c0a-be33-a6705d69c4cf&amp;pf_rd_r=4NMH6EWWFZNESEGGZP2H&amp;pid=bpmk5Iy&amp;qid=1701126928&amp;refinements=p_n_feature_twenty-three_browse-bin%3A19047482011%2Cp_n_feature_twenty-eight_browse-bin%3A19043709011%7C19043720011&amp;s=industrial&amp;sprefix=pcb%2Bstandoff%2Caps%2C124&amp;sr=1-3</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/10-10-32-Socket-Thermal-MonsterBolts/dp/B07CF7YD4W/ref=sr_1_4?content-id=amzn1.sym.918a99dd-4826-4c0a-be33-a6705d69c4cf%3Aamzn1.sym.918a99dd-4826-4c0a-be33-a6705d69c4cf&amp;crid=1TDVRIRN163RI&amp;keywords=Screws&amp;pd_rd_r=97bcc176-c819-4481-a510-9b05f5075494&amp;pd_rd_w=ZsYhC&amp;pd_rd_wg=kwwLA&amp;pf_rd_p=918a99dd-4826-4c0a-be33-a6705d69c4cf&amp;pf_rd_r=236WKXS83M80S8024RAW&amp;pid=rK5Vji9&amp;qid=1701127003&amp;refinements=p_n_feature_fourteen_browse-bin%3A11433964011%2Cp_n_feature_twenty-eight_browse-bin%3A19043652011&amp;s=industrial&amp;sprefix=10-32%2Bscrew%2Cindustrial%2C139&amp;sr=1-4&amp;th=1</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +193,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,20 +486,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.3125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.47265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,112 +515,217 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2" s="3">
+        <f>29*2</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>8</v>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>17</v>
+      <c r="D10" t="s">
+        <v>29</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
       </c>
       <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>19</v>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="4">
+        <f>SUM(F2:F12)</f>
+        <v>95.5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{31C23CB5-34AA-4098-BF96-69D3BD4C1292}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{48F9A34E-5952-4A05-A2AC-54EA8590386B}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{16E01F94-50EE-4680-A5BC-78B4B02B4B7E}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{C9F3E123-0834-4D93-91A1-6A0551EC7F1C}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{8F739283-135E-4CF3-B85C-5EB4771E9E1D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -564,10 +745,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -575,7 +756,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -583,7 +764,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -606,10 +787,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>

</xml_diff>